<commit_message>
source data (layers) were updated also extracting all patch areas
</commit_message>
<xml_diff>
--- a/Output/results_table.xlsx
+++ b/Output/results_table.xlsx
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="39" r:id="rId4"/>
+    <pivotCache cacheId="54" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
   <si>
     <t>unit</t>
   </si>
@@ -115,10 +115,16 @@
     <t>arid_south</t>
   </si>
   <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
     <t>Sum of p_area_mn</t>
   </si>
   <si>
     <t>average</t>
+  </si>
+  <si>
+    <t>Sum of unit_total_area_km2</t>
   </si>
 </sst>
 </file>
@@ -702,1447 +708,6 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
-  <c:pivotSource>
-    <c:name>[results_table.xlsx]Sheet2!PivotTable2</c:name>
-    <c:fmtId val="0"/>
-  </c:pivotSource>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="2"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="3"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="4"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="5"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="6"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="7"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="8"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="9"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="10"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="11"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="12"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="13"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="14"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="15"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="16"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="17"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="18"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="19"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="20"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="21"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="22"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="23"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="24"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="25"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="26"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="27"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="28"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="29"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="30"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="31"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="32"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="33"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="34"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="35"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="36"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="37"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="38"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$B$3:$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>arid_south</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$A$5:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$B$5:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>3.8567743750000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.83926945058997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.3465207443563099</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D399-4DE4-A1D7-F6C536BF7D9D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$C$3:$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>batha</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$A$5:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$C$5:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.84870306879496404</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.79617758985200804</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.74810561630218697</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D399-4DE4-A1D7-F6C536BF7D9D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$D$3:$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>coastal_sands</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$A$5:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$D$5:$D$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.147540716612378</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.140595238095238</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.13237406716417899</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D399-4DE4-A1D7-F6C536BF7D9D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$E$3:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>conifer_forest</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$A$5:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$E$5:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.120682882414152</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.11934907908294699</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.112841621588394</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D399-4DE4-A1D7-F6C536BF7D9D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$F$3:$F$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>desert_med_trans</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$A$5:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$F$5:$F$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.77691238584474898</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.73271802325581403</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.47681748792956602</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-D399-4DE4-A1D7-F6C536BF7D9D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$G$3:$G$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>inland_sands</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$A$5:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$G$5:$G$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>6.4608564814814802</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.4989091614906798</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.3417247191011201</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-D399-4DE4-A1D7-F6C536BF7D9D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$H$3:$H$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>loess</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$A$5:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$H$5:$H$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.73588541666666696</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.61978718199608596</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.50543609324758798</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-D399-4DE4-A1D7-F6C536BF7D9D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$I$3:$I$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>maquis</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$A$5:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$I$5:$I$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.206205755339196</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.19646270772091901</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.16684336467723601</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-D399-4DE4-A1D7-F6C536BF7D9D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$J$3:$J$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>negev_highlands</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$A$5:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$J$5:$J$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>7.2990816517189803</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.7507105809128598</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.6625191387559797</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-D399-4DE4-A1D7-F6C536BF7D9D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="460458352"/>
-        <c:axId val="460459664"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="460458352"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="460459664"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="460459664"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="460458352"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:extLst>
-    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
-      <c14:pivotOptions>
-        <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZoneSeries val="1"/>
-        <c14:dropZonesVisible val="1"/>
-      </c14:pivotOptions>
-    </c:ext>
-    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
-      <c16:pivotOptions16>
-        <c16:showExpandCollapseFieldButtons val="1"/>
-      </c16:pivotOptions16>
-    </c:ext>
-  </c:extLst>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:layout/>
@@ -3129,46 +1694,6 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3724,571 +2249,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>261939</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>61913</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>577850</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>42863</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>53975</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>79374</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>358775</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>60325</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>578555</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>49388</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4311,7 +2285,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Ron Chen" refreshedDate="44713.426661226855" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Ron Chen" refreshedDate="44713.468859722219" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
     <cacheField name="[Range].[unit].[unit]" caption="unit" numFmtId="0" level="1">
@@ -4343,9 +2317,9 @@
         </ext>
       </extLst>
     </cacheField>
-    <cacheField name="[Measures].[Sum of p_area_mn]" caption="Sum of p_area_mn" numFmtId="0" hierarchy="11" level="32767"/>
+    <cacheField name="[Measures].[Sum of unit_total_area_km2]" caption="Sum of unit_total_area_km2" numFmtId="0" hierarchy="12" level="32767"/>
   </cacheFields>
-  <cacheHierarchies count="12">
+  <cacheHierarchies count="13">
     <cacheHierarchy uniqueName="[Range].[unit]" caption="unit" attribute="1" defaultMemberUniqueName="[Range].[unit].[All]" allUniqueName="[Range].[unit].[All]" dimensionUniqueName="[Range]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
@@ -4367,13 +2341,20 @@
     <cacheHierarchy uniqueName="[Range].[unit_total_area_km2]" caption="unit_total_area_km2" attribute="1" defaultMemberUniqueName="[Range].[unit_total_area_km2].[All]" allUniqueName="[Range].[unit_total_area_km2].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Measures].[__XL_Count Range]" caption="__XL_Count Range" measure="1" displayFolder="" measureGroup="Range" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Sum of p_area_mn]" caption="Sum of p_area_mn" measure="1" displayFolder="" measureGroup="Range" count="0" oneField="1" hidden="1">
+    <cacheHierarchy uniqueName="[Measures].[Sum of p_area_mn]" caption="Sum of p_area_mn" measure="1" displayFolder="" measureGroup="Range" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="2"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of unit_total_area_km2]" caption="Sum of unit_total_area_km2" measure="1" displayFolder="" measureGroup="Range" count="0" oneField="1" hidden="1">
       <fieldsUsage count="1">
         <fieldUsage x="2"/>
       </fieldsUsage>
       <extLst>
         <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
-          <x15:cacheHierarchy aggregatedColumn="2"/>
+          <x15:cacheHierarchy aggregatedColumn="8"/>
         </ext>
       </extLst>
     </cacheHierarchy>
@@ -4398,8 +2379,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:J7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:K8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="10">
@@ -4428,7 +2409,7 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="4">
     <i>
       <x/>
     </i>
@@ -4438,11 +2419,14 @@
     <i>
       <x v="2"/>
     </i>
+    <i t="grand">
+      <x/>
+    </i>
   </rowItems>
   <colFields count="1">
     <field x="0"/>
   </colFields>
-  <colItems count="9">
+  <colItems count="10">
     <i>
       <x/>
     </i>
@@ -4470,417 +2454,75 @@
     <i>
       <x v="8"/>
     </i>
+    <i t="grand">
+      <x/>
+    </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of p_area_mn" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="Sum of unit_total_area_km2" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="36">
-    <chartFormat chart="0" format="3" series="1">
+  <chartFormats count="9">
+    <chartFormat chart="0" format="39" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="0" count="1" selected="0">
             <x v="4"/>
           </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="5" series="1">
+    <chartFormat chart="0" format="40" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="0" count="1" selected="0">
             <x v="5"/>
           </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="6" series="1">
+    <chartFormat chart="0" format="41" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="0" count="1" selected="0">
             <x v="6"/>
           </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="7" series="1">
+    <chartFormat chart="0" format="42" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="0" count="1" selected="0">
             <x v="7"/>
           </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
+    <chartFormat chart="0" format="43" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="0" count="1" selected="0">
             <x v="8"/>
           </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="11" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="12" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="15" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="16" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="17" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="18" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="19" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="20" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="21" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="22" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="23" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="24" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="25" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="26" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="27" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="28" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="29" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="30" series="1">
+    <chartFormat chart="0" format="44" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -4892,7 +2534,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="31" series="1">
+    <chartFormat chart="0" format="45" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -4904,7 +2546,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="32" series="1">
+    <chartFormat chart="0" format="46" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -4916,7 +2558,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="33" series="1">
+    <chartFormat chart="0" format="47" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -4928,68 +2570,8 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="34" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="35" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="36" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="37" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="38" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
   </chartFormats>
-  <pivotHierarchies count="12">
+  <pivotHierarchies count="13">
     <pivotHierarchy dragToData="1"/>
     <pivotHierarchy dragToData="1"/>
     <pivotHierarchy dragToData="1"/>
@@ -5001,6 +2583,7 @@
     <pivotHierarchy dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
     <pivotHierarchy dragToData="1"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -6111,7 +3694,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J7"/>
+  <dimension ref="A3:K8"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:J7"/>
@@ -6119,21 +3702,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.26953125" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.90625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16.36328125" bestFit="1" customWidth="1"/>
@@ -6143,12 +3732,12 @@
     <col min="32" max="32" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -6176,106 +3765,152 @@
       <c r="J4" t="s">
         <v>12</v>
       </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2015</v>
       </c>
       <c r="B5" s="3">
-        <v>3.8567743750000001</v>
+        <v>3956.1174999999998</v>
       </c>
       <c r="C5" s="3">
-        <v>0.84870306879496404</v>
+        <v>2076.7312499999998</v>
       </c>
       <c r="D5" s="3">
-        <v>0.147540716612378</v>
+        <v>344.07749999999999</v>
       </c>
       <c r="E5" s="3">
-        <v>0.120682882414152</v>
+        <v>488.50062500000001</v>
       </c>
       <c r="F5" s="3">
-        <v>0.77691238584474898</v>
+        <v>1949.8724999999999</v>
       </c>
       <c r="G5" s="3">
-        <v>6.4608564814814802</v>
+        <v>1075.9993750000001</v>
       </c>
       <c r="H5" s="3">
-        <v>0.73588541666666696</v>
+        <v>400.0675</v>
       </c>
       <c r="I5" s="3">
-        <v>0.206205755339196</v>
+        <v>4601.4925000000003</v>
       </c>
       <c r="J5" s="3">
-        <v>7.2990816517189803</v>
+        <v>5016.7924999999996</v>
+      </c>
+      <c r="K5" s="3">
+        <v>19909.651249999999</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>2017</v>
       </c>
       <c r="B6" s="3">
-        <v>2.83926945058997</v>
+        <v>3956.1174999999998</v>
       </c>
       <c r="C6" s="3">
-        <v>0.79617758985200804</v>
+        <v>2076.7312499999998</v>
       </c>
       <c r="D6" s="3">
-        <v>0.140595238095238</v>
+        <v>344.07749999999999</v>
       </c>
       <c r="E6" s="3">
-        <v>0.11934907908294699</v>
+        <v>488.50062500000001</v>
       </c>
       <c r="F6" s="3">
-        <v>0.73271802325581403</v>
+        <v>1949.8724999999999</v>
       </c>
       <c r="G6" s="3">
-        <v>6.4989091614906798</v>
+        <v>1075.9993750000001</v>
       </c>
       <c r="H6" s="3">
-        <v>0.61978718199608596</v>
+        <v>400.0675</v>
       </c>
       <c r="I6" s="3">
-        <v>0.19646270772091901</v>
+        <v>4601.4925000000003</v>
       </c>
       <c r="J6" s="3">
-        <v>6.7507105809128598</v>
+        <v>5016.7924999999996</v>
+      </c>
+      <c r="K6" s="3">
+        <v>19909.651249999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>2020</v>
       </c>
       <c r="B7" s="3">
-        <v>2.3465207443563099</v>
+        <v>3956.1174999999998</v>
       </c>
       <c r="C7" s="3">
-        <v>0.74810561630218697</v>
+        <v>2076.7312499999998</v>
       </c>
       <c r="D7" s="3">
-        <v>0.13237406716417899</v>
+        <v>344.07749999999999</v>
       </c>
       <c r="E7" s="3">
-        <v>0.112841621588394</v>
+        <v>488.50062500000001</v>
       </c>
       <c r="F7" s="3">
-        <v>0.47681748792956602</v>
+        <v>1949.8724999999999</v>
       </c>
       <c r="G7" s="3">
-        <v>2.3417247191011201</v>
+        <v>1075.9993750000001</v>
       </c>
       <c r="H7" s="3">
-        <v>0.50543609324758798</v>
+        <v>400.0675</v>
       </c>
       <c r="I7" s="3">
-        <v>0.16684336467723601</v>
+        <v>4601.4925000000003</v>
       </c>
       <c r="J7" s="3">
-        <v>4.6625191387559797</v>
+        <v>5016.7924999999996</v>
+      </c>
+      <c r="K7" s="3">
+        <v>19909.651249999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3">
+        <v>11868.352499999999</v>
+      </c>
+      <c r="C8" s="3">
+        <v>6230.1937499999995</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1032.2325000000001</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1465.5018749999999</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5849.6175000000003</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3227.9981250000001</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1200.2024999999999</v>
+      </c>
+      <c r="I8" s="3">
+        <v>13804.477500000001</v>
+      </c>
+      <c r="J8" s="3">
+        <v>15050.377499999999</v>
+      </c>
+      <c r="K8" s="3">
+        <v>59728.953749999986</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6283,7 +3918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -6291,7 +3926,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -6448,7 +4083,7 @@
         <v>12</v>
       </c>
       <c r="K7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>